<commit_message>
Modificación xlsx prueba de pestaña TM en formato
</commit_message>
<xml_diff>
--- a/PruebasFuncionales_CuadroMando/PruebaCuadroMando_TM.xlsx
+++ b/PruebasFuncionales_CuadroMando/PruebaCuadroMando_TM.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jruizarr\Desktop\Pruebas cuadro de mando\TM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Documents\BlackMargin\MarginBlack\PruebasFuncionales_CuadroMando\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="7260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9580" windowHeight="7260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RESUMEN" sheetId="1" r:id="rId1"/>
     <sheet name="Prueba 1" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Prueba 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -97,7 +97,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -105,22 +105,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,56 +624,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -694,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>